<commit_message>
Added ifo Forecast Enhancement Module
</commit_message>
<xml_diff>
--- a/0_0_Data/0_Forecast_Inputs/2_ifoCAST/ifoCAST_nowcasts_full.xlsx
+++ b/0_0_Data/0_Forecast_Inputs/2_ifoCAST/ifoCAST_nowcasts_full.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/0_0_Data/0_Forecast_Inputs/2_ifoCAST/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_277C25313431921FD2FE31D2F87AE380480137E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EC5B5F6-A47A-46F2-B6FA-EF571F60399F}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -25,11 +31,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,17 +97,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -139,7 +153,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -173,6 +187,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -207,9 +222,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -382,14 +398,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -397,23 +416,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>40403</v>
       </c>
       <c r="B2">
-        <v>0.241766699317489</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>0.24176669931748901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>40494</v>
       </c>
       <c r="B3">
-        <v>0.444900743380838</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>0.44490074338083802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>40589</v>
       </c>
@@ -421,47 +440,47 @@
         <v>1.10047060058947</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>40676</v>
       </c>
       <c r="B5">
-        <v>0.352879089972535</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>0.35287908997253498</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>40771</v>
       </c>
       <c r="B6">
-        <v>0.747708439466207</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>0.74770843946620702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>40862</v>
       </c>
       <c r="B7">
-        <v>0.231784144206971</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>0.23178414420697099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>40954</v>
       </c>
       <c r="B8">
-        <v>-0.0705000780773346</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>-7.0500078077334605E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>41044</v>
       </c>
       <c r="B9">
-        <v>-0.137004828987682</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>-0.13700482898768199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>41135</v>
       </c>
@@ -469,15 +488,15 @@
         <v>0.170928318082751</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>41228</v>
       </c>
       <c r="B11">
-        <v>-0.09251056768275739</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>-9.2510567682757394E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>41319</v>
       </c>
@@ -485,55 +504,55 @@
         <v>0.109019749499752</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>41409</v>
       </c>
       <c r="B13">
-        <v>0.535895844045383</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>0.53589584404538304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>41500</v>
       </c>
       <c r="B14">
-        <v>0.0480574359319111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>4.8057435931911099E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>41592</v>
       </c>
       <c r="B15">
-        <v>0.336410475895099</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>0.33641047589509898</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>41684</v>
       </c>
       <c r="B16">
-        <v>1.15648798444962</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>1.1564879844496201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>41774</v>
       </c>
       <c r="B17">
-        <v>0.0917580682271779</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>9.17580682271779E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>41865</v>
       </c>
       <c r="B18">
-        <v>0.432960026496128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>0.43296002649612803</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>41957</v>
       </c>
@@ -541,55 +560,55 @@
         <v>0.406193507823847</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>42048</v>
       </c>
       <c r="B20">
-        <v>0.678223131929459</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>0.67822313192945904</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>42137</v>
       </c>
       <c r="B21">
-        <v>0.480124956126704</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>0.48012495612670397</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>42230</v>
       </c>
       <c r="B22">
-        <v>0.63387961181501</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>0.63387961181500996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>42321</v>
       </c>
       <c r="B23">
-        <v>0.395376664579939</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>0.39537666457993897</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>42412</v>
       </c>
       <c r="B24">
-        <v>0.525521119631444</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>0.52552111963144399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>42503</v>
       </c>
       <c r="B25">
-        <v>0.350906646240513</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>0.35090664624051299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>42594</v>
       </c>
@@ -597,7 +616,7 @@
         <v>-0.121181656452894</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>42689</v>
       </c>
@@ -605,63 +624,63 @@
         <v>1.12101181637889</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>42780</v>
       </c>
       <c r="B28">
-        <v>0.541918428615552</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>0.54191842861555195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>42867</v>
       </c>
       <c r="B29">
-        <v>0.809577098583235</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>0.80957709858323501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>42962</v>
       </c>
       <c r="B30">
-        <v>0.381733395966201</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>0.38173339596620098</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>43053</v>
       </c>
       <c r="B31">
-        <v>0.515056337211413</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>0.51505633721141297</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>43145</v>
       </c>
       <c r="B32">
-        <v>0.541582629209194</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>0.54158262920919398</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>43235</v>
       </c>
       <c r="B33">
-        <v>-0.138856201462895</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>-0.13885620146289501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>43326</v>
       </c>
       <c r="B34">
-        <v>0.0503775864399945</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>5.0377586439994501E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>43418</v>
       </c>
@@ -669,63 +688,63 @@
         <v>0.24747400421905</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>43510</v>
       </c>
       <c r="B36">
-        <v>0.601318885903152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>0.60131888590315197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>43600</v>
       </c>
       <c r="B37">
-        <v>-0.302587196304716</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>-0.30258719630471598</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>43691</v>
       </c>
       <c r="B38">
-        <v>0.235914458649045</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>0.23591445864904501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>43783</v>
       </c>
       <c r="B39">
-        <v>0.024124257856421</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>2.4124257856421E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>43909</v>
       </c>
       <c r="B40">
-        <v>0.7155752359999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>0.71557523599999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>44011</v>
       </c>
       <c r="B41">
-        <v>-7.451780981</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>-7.4517809809999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>44096</v>
       </c>
       <c r="B42">
-        <v>6.405694238</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>6.4056942379999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>44181</v>
       </c>
@@ -733,23 +752,23 @@
         <v>-1.14456628109437</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>44279</v>
       </c>
       <c r="B44">
-        <v>1.297172517</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>1.2971725169999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>44363</v>
       </c>
       <c r="B45">
-        <v>0.673905569079516</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>0.67390556907951604</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>44461</v>
       </c>
@@ -757,79 +776,79 @@
         <v>0.347602564</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>44544</v>
       </c>
       <c r="B47">
-        <v>-0.24627924</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>-0.24627924000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>44643</v>
       </c>
       <c r="B48">
-        <v>2.276288116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>2.2762881159999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>44727</v>
       </c>
       <c r="B49">
-        <v>0.92820296</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>0.92820296000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>44816</v>
       </c>
       <c r="B50">
-        <v>-0.277926312</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>-0.27792631200000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>44909</v>
       </c>
       <c r="B51">
-        <v>0.251316528</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>0.25131652799999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>45000</v>
       </c>
       <c r="B52">
-        <v>0.538736913</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>0.53873691300000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>45098</v>
       </c>
       <c r="B53">
-        <v>-0.318864405</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>-0.31886440500000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>45176</v>
       </c>
       <c r="B54">
-        <v>-0.474503149</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>-0.47450314900000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>45274</v>
       </c>
       <c r="B55">
-        <v>-0.290614742754258</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>-0.29061474275425803</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>45357</v>
       </c>
@@ -837,52 +856,52 @@
         <v>-0.236658442</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>45463</v>
       </c>
       <c r="B57">
-        <v>0.374912587</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>0.37491258700000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>45540</v>
       </c>
       <c r="B58">
-        <v>-0.559269386</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>-0.55926938599999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>45638</v>
       </c>
       <c r="B59">
-        <v>0.135411462</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>0.13541146200000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>45733</v>
       </c>
       <c r="B60">
-        <v>0.332099825</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>0.33209982500000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>45820</v>
       </c>
       <c r="B61">
-        <v>0.028721274</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>2.8721274000000001E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>45904</v>
       </c>
       <c r="B62">
-        <v>0.042359665</v>
+        <v>4.2359664999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added filtering options for the Component Analysis
</commit_message>
<xml_diff>
--- a/0_0_Data/0_Forecast_Inputs/2_ifoCAST/ifoCAST_nowcasts_full.xlsx
+++ b/0_0_Data/0_Forecast_Inputs/2_ifoCAST/ifoCAST_nowcasts_full.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/0_0_Data/0_Forecast_Inputs/2_ifoCAST/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_277C25313431921FD2FE31D2F87AE380480137E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EC5B5F6-A47A-46F2-B6FA-EF571F60399F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -31,11 +25,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,25 +91,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,7 +139,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -187,7 +173,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -222,10 +207,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -398,17 +382,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="31.1796875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -416,23 +397,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>40403</v>
       </c>
       <c r="B2">
-        <v>0.24176669931748901</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.241766699317489</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>40494</v>
       </c>
       <c r="B3">
-        <v>0.44490074338083802</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.444900743380838</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>40589</v>
       </c>
@@ -440,47 +421,47 @@
         <v>1.10047060058947</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>40676</v>
       </c>
       <c r="B5">
-        <v>0.35287908997253498</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.352879089972535</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>40771</v>
       </c>
       <c r="B6">
-        <v>0.74770843946620702</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.747708439466207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>40862</v>
       </c>
       <c r="B7">
-        <v>0.23178414420697099</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.231784144206971</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>40954</v>
       </c>
       <c r="B8">
-        <v>-7.0500078077334605E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.0705000780773346</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="2">
         <v>41044</v>
       </c>
       <c r="B9">
-        <v>-0.13700482898768199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.137004828987682</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>41135</v>
       </c>
@@ -488,15 +469,15 @@
         <v>0.170928318082751</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>41228</v>
       </c>
       <c r="B11">
-        <v>-9.2510567682757394E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.09251056768275739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="2">
         <v>41319</v>
       </c>
@@ -504,55 +485,55 @@
         <v>0.109019749499752</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>41409</v>
       </c>
       <c r="B13">
-        <v>0.53589584404538304</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.535895844045383</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>41500</v>
       </c>
       <c r="B14">
-        <v>4.8057435931911099E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.0480574359319111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="2">
         <v>41592</v>
       </c>
       <c r="B15">
-        <v>0.33641047589509898</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.336410475895099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="2">
         <v>41684</v>
       </c>
       <c r="B16">
-        <v>1.1564879844496201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.15648798444962</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="2">
         <v>41774</v>
       </c>
       <c r="B17">
-        <v>9.17580682271779E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.0917580682271779</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="2">
         <v>41865</v>
       </c>
       <c r="B18">
-        <v>0.43296002649612803</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.432960026496128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="2">
         <v>41957</v>
       </c>
@@ -560,55 +541,55 @@
         <v>0.406193507823847</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2">
       <c r="A20" s="2">
         <v>42048</v>
       </c>
       <c r="B20">
-        <v>0.67822313192945904</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.678223131929459</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="2">
         <v>42137</v>
       </c>
       <c r="B21">
-        <v>0.48012495612670397</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.480124956126704</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="2">
         <v>42230</v>
       </c>
       <c r="B22">
-        <v>0.63387961181500996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.63387961181501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="2">
         <v>42321</v>
       </c>
       <c r="B23">
-        <v>0.39537666457993897</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.395376664579939</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="2">
         <v>42412</v>
       </c>
       <c r="B24">
-        <v>0.52552111963144399</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.525521119631444</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="2">
         <v>42503</v>
       </c>
       <c r="B25">
-        <v>0.35090664624051299</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.350906646240513</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="2">
         <v>42594</v>
       </c>
@@ -616,7 +597,7 @@
         <v>-0.121181656452894</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2">
       <c r="A27" s="2">
         <v>42689</v>
       </c>
@@ -624,63 +605,63 @@
         <v>1.12101181637889</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2">
       <c r="A28" s="2">
         <v>42780</v>
       </c>
       <c r="B28">
-        <v>0.54191842861555195</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.541918428615552</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="2">
         <v>42867</v>
       </c>
       <c r="B29">
-        <v>0.80957709858323501</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.809577098583235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="2">
         <v>42962</v>
       </c>
       <c r="B30">
-        <v>0.38173339596620098</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.381733395966201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="2">
         <v>43053</v>
       </c>
       <c r="B31">
-        <v>0.51505633721141297</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.515056337211413</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="2">
         <v>43145</v>
       </c>
       <c r="B32">
-        <v>0.54158262920919398</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.541582629209194</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="2">
         <v>43235</v>
       </c>
       <c r="B33">
-        <v>-0.13885620146289501</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.138856201462895</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="2">
         <v>43326</v>
       </c>
       <c r="B34">
-        <v>5.0377586439994501E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.0503775864399945</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="2">
         <v>43418</v>
       </c>
@@ -688,63 +669,63 @@
         <v>0.24747400421905</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2">
       <c r="A36" s="2">
         <v>43510</v>
       </c>
       <c r="B36">
-        <v>0.60131888590315197</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.601318885903152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="2">
         <v>43600</v>
       </c>
       <c r="B37">
-        <v>-0.30258719630471598</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.302587196304716</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="2">
         <v>43691</v>
       </c>
       <c r="B38">
-        <v>0.23591445864904501</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.235914458649045</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="2">
         <v>43783</v>
       </c>
       <c r="B39">
-        <v>2.4124257856421E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.024124257856421</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="2">
         <v>43909</v>
       </c>
       <c r="B40">
-        <v>0.71557523599999995</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.7155752359999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="2">
         <v>44011</v>
       </c>
       <c r="B41">
-        <v>-7.4517809809999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-7.451780981</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="2">
         <v>44096</v>
       </c>
       <c r="B42">
-        <v>6.4056942379999997</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+        <v>6.405694238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="2">
         <v>44181</v>
       </c>
@@ -752,23 +733,23 @@
         <v>-1.14456628109437</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2">
       <c r="A44" s="2">
         <v>44279</v>
       </c>
       <c r="B44">
-        <v>1.2971725169999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1.297172517</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="2">
         <v>44363</v>
       </c>
       <c r="B45">
-        <v>0.67390556907951604</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.673905569079516</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="2">
         <v>44461</v>
       </c>
@@ -776,79 +757,79 @@
         <v>0.347602564</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2">
       <c r="A47" s="2">
         <v>44544</v>
       </c>
       <c r="B47">
-        <v>-0.24627924000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.24627924</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="2">
         <v>44643</v>
       </c>
       <c r="B48">
-        <v>2.2762881159999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2.276288116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="2">
         <v>44727</v>
       </c>
       <c r="B49">
-        <v>0.92820296000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.92820296</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" s="2">
         <v>44816</v>
       </c>
       <c r="B50">
-        <v>-0.27792631200000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.277926312</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" s="2">
         <v>44909</v>
       </c>
       <c r="B51">
-        <v>0.25131652799999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.251316528</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" s="2">
         <v>45000</v>
       </c>
       <c r="B52">
-        <v>0.53873691300000004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.538736913</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" s="2">
         <v>45098</v>
       </c>
       <c r="B53">
-        <v>-0.31886440500000002</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.318864405</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" s="2">
         <v>45176</v>
       </c>
       <c r="B54">
-        <v>-0.47450314900000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.474503149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" s="2">
         <v>45274</v>
       </c>
       <c r="B55">
-        <v>-0.29061474275425803</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.290614742754258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" s="2">
         <v>45357</v>
       </c>
@@ -856,52 +837,52 @@
         <v>-0.236658442</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2">
       <c r="A57" s="2">
         <v>45463</v>
       </c>
       <c r="B57">
-        <v>0.37491258700000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.374912587</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" s="2">
         <v>45540</v>
       </c>
       <c r="B58">
-        <v>-0.55926938599999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+        <v>-0.559269386</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" s="2">
         <v>45638</v>
       </c>
       <c r="B59">
-        <v>0.13541146200000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.135411462</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" s="2">
         <v>45733</v>
       </c>
       <c r="B60">
-        <v>0.33209982500000002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.332099825</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="2">
         <v>45820</v>
       </c>
       <c r="B61">
-        <v>2.8721274000000001E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0.028721274</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" s="2">
         <v>45904</v>
       </c>
       <c r="B62">
-        <v>4.2359664999999998E-2</v>
+        <v>0.042359665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>